<commit_message>
testing calibration run retail_ideal_calibration.xlsx
</commit_message>
<xml_diff>
--- a/projects/retail_optim2.xlsx
+++ b/projects/retail_optim2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16440" tabRatio="562" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -6373,8 +6373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6654,7 +6654,7 @@
         <v>559</v>
       </c>
       <c r="B26" s="29">
-        <v>45036000000000</v>
+        <v>450360000000000</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>577</v>
@@ -8996,9 +8996,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>